<commit_message>
Update bidouille club modif Steph riri plus.xlsx
</commit_message>
<xml_diff>
--- a/Console_DMX_html_VS_1_esp32/bidouille club modif Steph riri plus.xlsx
+++ b/Console_DMX_html_VS_1_esp32/bidouille club modif Steph riri plus.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="127">
   <si>
     <t xml:space="preserve">R</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t xml:space="preserve">medza D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route</t>
   </si>
   <si>
     <t xml:space="preserve">r</t>
@@ -409,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -431,12 +434,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="16">
@@ -531,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -703,6 +700,13 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
       <top style="medium"/>
       <bottom style="medium"/>
       <diagonal/>
@@ -757,7 +761,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="142">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -790,10 +794,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1130,7 +1130,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1162,15 +1162,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1186,43 +1182,63 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="15" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1254,11 +1270,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1266,6 +1278,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1298,7 +1314,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1395,10 +1411,10 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="1" sqref="E27:E28 F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="16"/>
@@ -1600,13 +1616,13 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="1" sqref="E27:E28 I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="18.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8"/>
@@ -1638,10 +1654,10 @@
       <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1649,22 +1665,22 @@
       <c r="A2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1672,22 +1688,22 @@
       <c r="A3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="9" t="n">
+      <c r="B3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14" t="s">
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1695,34 +1711,34 @@
       <c r="A4" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="15" t="n">
+      <c r="B4" s="14" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="19" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1730,7 +1746,7 @@
       <c r="A5" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="21" t="n">
+      <c r="B5" s="20" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1745,15 +1761,15 @@
       <c r="F5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="2" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1761,30 +1777,30 @@
       <c r="A6" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="26" t="n">
+      <c r="D6" s="25" t="n">
         <v>32</v>
       </c>
-      <c r="E6" s="26" t="n">
+      <c r="E6" s="25" t="n">
         <v>33</v>
       </c>
-      <c r="F6" s="26" t="n">
+      <c r="F6" s="25" t="n">
         <v>34</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28" t="n">
+      <c r="G6" s="26"/>
+      <c r="H6" s="27" t="n">
         <v>31</v>
       </c>
-      <c r="I6" s="29" t="n">
+      <c r="I6" s="28" t="n">
         <v>36</v>
       </c>
-      <c r="J6" s="30" t="n">
+      <c r="J6" s="29" t="n">
         <v>37</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="29" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1792,30 +1808,30 @@
       <c r="A7" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="26" t="n">
+      <c r="D7" s="25" t="n">
         <v>25</v>
       </c>
-      <c r="E7" s="26" t="n">
+      <c r="E7" s="25" t="n">
         <v>26</v>
       </c>
-      <c r="F7" s="26" t="n">
+      <c r="F7" s="25" t="n">
         <v>27</v>
       </c>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28" t="n">
+      <c r="G7" s="26"/>
+      <c r="H7" s="27" t="n">
         <v>24</v>
       </c>
-      <c r="I7" s="29" t="n">
+      <c r="I7" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="J7" s="30" t="n">
+      <c r="J7" s="29" t="n">
         <v>30</v>
       </c>
-      <c r="K7" s="30" t="s">
+      <c r="K7" s="29" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1823,34 +1839,34 @@
       <c r="A8" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="15" t="n">
+      <c r="B8" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="19" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1858,34 +1874,34 @@
       <c r="A9" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="31" t="n">
+      <c r="B9" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="32" t="n">
+      <c r="E9" s="31" t="n">
         <v>173.181</v>
       </c>
-      <c r="F9" s="32" t="n">
+      <c r="F9" s="31" t="n">
         <v>174.182</v>
       </c>
-      <c r="G9" s="33" t="n">
+      <c r="G9" s="32" t="n">
         <v>175.183</v>
       </c>
-      <c r="H9" s="34" t="n">
+      <c r="H9" s="33" t="n">
         <v>171.179</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="36" t="s">
+      <c r="J9" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="35" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1893,34 +1909,34 @@
       <c r="A10" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="31" t="n">
+      <c r="B10" s="30" t="n">
         <v>7</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="32" t="n">
+      <c r="D10" s="31" t="n">
         <v>188</v>
       </c>
-      <c r="E10" s="32" t="n">
+      <c r="E10" s="31" t="n">
         <v>189</v>
       </c>
-      <c r="F10" s="32" t="n">
+      <c r="F10" s="31" t="n">
         <v>190</v>
       </c>
-      <c r="G10" s="33" t="n">
+      <c r="G10" s="32" t="n">
         <v>191</v>
       </c>
-      <c r="H10" s="34" t="n">
+      <c r="H10" s="33" t="n">
         <v>187</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="36" t="s">
+      <c r="K10" s="35" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1928,34 +1944,34 @@
       <c r="A11" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="31" t="n">
+      <c r="B11" s="30" t="n">
         <v>8</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="32" t="n">
+      <c r="D11" s="31" t="n">
         <v>196</v>
       </c>
-      <c r="E11" s="32" t="n">
+      <c r="E11" s="31" t="n">
         <v>197</v>
       </c>
-      <c r="F11" s="32" t="n">
+      <c r="F11" s="31" t="n">
         <v>198</v>
       </c>
-      <c r="G11" s="33" t="n">
+      <c r="G11" s="32" t="n">
         <v>199</v>
       </c>
-      <c r="H11" s="34" t="n">
+      <c r="H11" s="33" t="n">
         <v>195</v>
       </c>
-      <c r="I11" s="35" t="s">
+      <c r="I11" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="35" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1963,34 +1979,34 @@
       <c r="A12" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="15" t="n">
+      <c r="B12" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="16" t="n">
+      <c r="D12" s="15" t="n">
         <v>102.112</v>
       </c>
-      <c r="E12" s="16" t="n">
+      <c r="E12" s="15" t="n">
         <v>103.113</v>
       </c>
-      <c r="F12" s="16" t="n">
+      <c r="F12" s="15" t="n">
         <v>104.114</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="37" t="n">
+      <c r="H12" s="36" t="n">
         <v>101.111</v>
       </c>
-      <c r="I12" s="19" t="n">
+      <c r="I12" s="18" t="n">
         <v>107.117</v>
       </c>
-      <c r="J12" s="20" t="n">
+      <c r="J12" s="19" t="n">
         <v>108.118</v>
       </c>
-      <c r="K12" s="20" t="s">
+      <c r="K12" s="19" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2016,10 +2032,10 @@
   <dimension ref="A1:Y48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q49" activeCellId="0" sqref="Q49"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E27:E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="n">
@@ -2031,198 +2047,198 @@
       <c r="C1" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D1" s="38" t="n">
+      <c r="D1" s="37" t="n">
         <v>4</v>
       </c>
-      <c r="E1" s="39" t="n">
+      <c r="E1" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="F1" s="40" t="n">
+      <c r="F1" s="39" t="n">
         <v>6</v>
       </c>
-      <c r="G1" s="41" t="n">
+      <c r="G1" s="40" t="n">
         <v>7</v>
       </c>
-      <c r="H1" s="39" t="n">
+      <c r="H1" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="I1" s="40" t="n">
+      <c r="I1" s="39" t="n">
         <v>9</v>
       </c>
-      <c r="J1" s="41" t="n">
+      <c r="J1" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="K1" s="39" t="n">
+      <c r="K1" s="38" t="n">
         <v>11</v>
       </c>
-      <c r="L1" s="40" t="n">
+      <c r="L1" s="39" t="n">
         <v>12</v>
       </c>
-      <c r="M1" s="41" t="n">
+      <c r="M1" s="40" t="n">
         <v>13</v>
       </c>
-      <c r="N1" s="39" t="n">
+      <c r="N1" s="38" t="n">
         <v>14</v>
       </c>
-      <c r="O1" s="42" t="n">
+      <c r="O1" s="41" t="n">
         <v>15</v>
       </c>
       <c r="P1" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="Q1" s="43" t="n">
+      <c r="Q1" s="42" t="n">
         <v>17</v>
       </c>
-      <c r="R1" s="44" t="n">
+      <c r="R1" s="43" t="n">
         <v>18</v>
       </c>
-      <c r="S1" s="36" t="n">
+      <c r="S1" s="35" t="n">
         <v>19</v>
       </c>
-      <c r="T1" s="45" t="n">
+      <c r="T1" s="44" t="n">
         <v>20</v>
       </c>
       <c r="U1" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="V1" s="46" t="n">
+      <c r="V1" s="45" t="n">
         <v>22</v>
       </c>
-      <c r="W1" s="47" t="n">
+      <c r="W1" s="46" t="n">
         <v>23</v>
       </c>
-      <c r="X1" s="48" t="n">
+      <c r="X1" s="47" t="n">
         <v>24</v>
       </c>
-      <c r="Y1" s="41" t="n">
+      <c r="Y1" s="40" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="55" t="s">
+      <c r="K2" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="53" t="s">
+      <c r="L2" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="54" t="s">
+      <c r="M2" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="O2" s="56" t="s">
+      <c r="O2" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="58" t="s">
+      <c r="P2" s="56"/>
+      <c r="Q2" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="R2" s="59" t="s">
+      <c r="R2" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="S2" s="52" t="s">
+      <c r="S2" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="T2" s="45" t="s">
+      <c r="T2" s="44" t="s">
         <v>85</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="V2" s="46" t="s">
+      <c r="V2" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="W2" s="47" t="s">
+      <c r="W2" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="X2" s="60" t="s">
+      <c r="X2" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="53" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="n">
+      <c r="A3" s="38" t="n">
         <v>26</v>
       </c>
-      <c r="B3" s="40" t="n">
+      <c r="B3" s="39" t="n">
         <v>27</v>
       </c>
-      <c r="C3" s="61" t="n">
+      <c r="C3" s="60" t="n">
         <v>28</v>
       </c>
-      <c r="D3" s="62" t="n">
+      <c r="D3" s="61" t="n">
         <v>29</v>
       </c>
-      <c r="E3" s="63" t="n">
+      <c r="E3" s="62" t="n">
         <v>30</v>
       </c>
-      <c r="F3" s="48" t="n">
+      <c r="F3" s="47" t="n">
         <v>31</v>
       </c>
-      <c r="G3" s="41" t="n">
+      <c r="G3" s="40" t="n">
         <v>32</v>
       </c>
-      <c r="H3" s="39" t="n">
+      <c r="H3" s="38" t="n">
         <v>33</v>
       </c>
-      <c r="I3" s="40" t="n">
+      <c r="I3" s="39" t="n">
         <v>34</v>
       </c>
-      <c r="J3" s="61" t="n">
+      <c r="J3" s="60" t="n">
         <v>35</v>
       </c>
-      <c r="K3" s="62" t="n">
+      <c r="K3" s="61" t="n">
         <v>36</v>
       </c>
-      <c r="L3" s="63" t="n">
+      <c r="L3" s="62" t="n">
         <v>37</v>
       </c>
-      <c r="M3" s="64" t="n">
+      <c r="M3" s="63" t="n">
         <v>38</v>
       </c>
-      <c r="N3" s="65" t="n">
+      <c r="N3" s="64" t="n">
         <v>39</v>
       </c>
-      <c r="O3" s="66" t="n">
+      <c r="O3" s="65" t="n">
         <v>40</v>
       </c>
-      <c r="P3" s="48" t="n">
+      <c r="P3" s="47" t="n">
         <v>41</v>
       </c>
-      <c r="Q3" s="67" t="n">
+      <c r="Q3" s="66" t="n">
         <v>42</v>
       </c>
-      <c r="R3" s="48" t="n">
+      <c r="R3" s="47" t="n">
         <v>43</v>
       </c>
-      <c r="S3" s="67" t="n">
+      <c r="S3" s="66" t="n">
         <v>44</v>
       </c>
       <c r="T3" s="7" t="n">
@@ -2237,1296 +2253,1312 @@
       <c r="W3" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="X3" s="65" t="n">
+      <c r="X3" s="64" t="n">
         <v>49</v>
       </c>
-      <c r="Y3" s="65" t="n">
+      <c r="Y3" s="64" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="4" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="59" t="s">
+      <c r="G4" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="72" t="s">
+      <c r="I4" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="L4" s="74" t="s">
+      <c r="L4" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="71" t="s">
+      <c r="M4" s="56"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="Q4" s="75" t="s">
+      <c r="Q4" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="R4" s="71" t="s">
+      <c r="R4" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="S4" s="75" t="s">
+      <c r="S4" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="49"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
     </row>
     <row r="5" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="n">
+      <c r="A5" s="47" t="n">
         <v>51</v>
       </c>
-      <c r="B5" s="41" t="n">
+      <c r="B5" s="40" t="n">
         <v>52</v>
       </c>
-      <c r="C5" s="39" t="n">
+      <c r="C5" s="38" t="n">
         <v>53</v>
       </c>
-      <c r="D5" s="40" t="n">
+      <c r="D5" s="39" t="n">
         <v>54</v>
       </c>
-      <c r="E5" s="61" t="n">
+      <c r="E5" s="60" t="n">
         <v>55</v>
       </c>
-      <c r="F5" s="61" t="n">
+      <c r="F5" s="60" t="n">
         <v>56</v>
       </c>
-      <c r="G5" s="62" t="n">
+      <c r="G5" s="61" t="n">
         <v>57</v>
       </c>
-      <c r="H5" s="76" t="n">
+      <c r="H5" s="75" t="n">
         <v>58</v>
       </c>
-      <c r="I5" s="61" t="n">
+      <c r="I5" s="60" t="n">
         <v>59</v>
       </c>
-      <c r="J5" s="77" t="n">
+      <c r="J5" s="76" t="n">
         <v>60</v>
       </c>
-      <c r="K5" s="48" t="n">
+      <c r="K5" s="47" t="n">
         <v>61</v>
       </c>
-      <c r="L5" s="41" t="n">
+      <c r="L5" s="40" t="n">
         <v>62</v>
       </c>
-      <c r="M5" s="39" t="n">
+      <c r="M5" s="38" t="n">
         <v>63</v>
       </c>
-      <c r="N5" s="40" t="n">
+      <c r="N5" s="39" t="n">
         <v>64</v>
       </c>
-      <c r="O5" s="61" t="n">
+      <c r="O5" s="60" t="n">
         <v>65</v>
       </c>
-      <c r="P5" s="61" t="n">
+      <c r="P5" s="60" t="n">
         <v>66</v>
       </c>
-      <c r="Q5" s="62" t="n">
+      <c r="Q5" s="61" t="n">
         <v>67</v>
       </c>
-      <c r="R5" s="61" t="n">
+      <c r="R5" s="60" t="n">
         <v>68</v>
       </c>
-      <c r="S5" s="61" t="n">
+      <c r="S5" s="60" t="n">
         <v>69</v>
       </c>
-      <c r="T5" s="77" t="n">
+      <c r="T5" s="76" t="n">
         <v>70</v>
       </c>
-      <c r="U5" s="48" t="n">
+      <c r="U5" s="47" t="n">
         <v>71</v>
       </c>
-      <c r="V5" s="41" t="n">
+      <c r="V5" s="40" t="n">
         <v>72</v>
       </c>
-      <c r="W5" s="39" t="n">
+      <c r="W5" s="38" t="n">
         <v>73</v>
       </c>
-      <c r="X5" s="40" t="n">
+      <c r="X5" s="39" t="n">
         <v>74</v>
       </c>
-      <c r="Y5" s="61" t="n">
+      <c r="Y5" s="60" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="6" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="N6" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="U6" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="W6" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y6" s="68" t="s">
+      <c r="A6" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="O6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y6" s="67" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="61" t="n">
+      <c r="A7" s="60" t="n">
         <v>76</v>
       </c>
-      <c r="B7" s="62" t="n">
+      <c r="B7" s="61" t="n">
         <v>77</v>
       </c>
-      <c r="C7" s="76" t="n">
+      <c r="C7" s="75" t="n">
         <v>78</v>
       </c>
-      <c r="D7" s="61" t="n">
+      <c r="D7" s="60" t="n">
         <v>79</v>
       </c>
-      <c r="E7" s="77" t="n">
+      <c r="E7" s="76" t="n">
         <v>80</v>
       </c>
-      <c r="F7" s="48" t="n">
+      <c r="F7" s="47" t="n">
         <v>81</v>
       </c>
-      <c r="G7" s="41" t="n">
+      <c r="G7" s="40" t="n">
         <v>82</v>
       </c>
-      <c r="H7" s="39" t="n">
+      <c r="H7" s="38" t="n">
         <v>83</v>
       </c>
-      <c r="I7" s="40" t="n">
+      <c r="I7" s="39" t="n">
         <v>84</v>
       </c>
-      <c r="J7" s="80" t="n">
+      <c r="J7" s="79" t="n">
         <v>85</v>
       </c>
-      <c r="K7" s="61" t="n">
+      <c r="K7" s="60" t="n">
         <v>86</v>
       </c>
-      <c r="L7" s="62" t="n">
+      <c r="L7" s="61" t="n">
         <v>87</v>
       </c>
-      <c r="M7" s="76" t="n">
-        <v>88</v>
-      </c>
-      <c r="N7" s="61" t="n">
+      <c r="M7" s="75" t="n">
+        <v>88</v>
+      </c>
+      <c r="N7" s="60" t="n">
         <v>89</v>
       </c>
-      <c r="O7" s="77" t="n">
+      <c r="O7" s="76" t="n">
         <v>90</v>
       </c>
-      <c r="P7" s="48" t="n">
+      <c r="P7" s="47" t="n">
         <v>91</v>
       </c>
-      <c r="Q7" s="41" t="n">
+      <c r="Q7" s="40" t="n">
         <v>92</v>
       </c>
-      <c r="R7" s="39" t="n">
+      <c r="R7" s="38" t="n">
         <v>93</v>
       </c>
-      <c r="S7" s="40" t="n">
+      <c r="S7" s="39" t="n">
         <v>94</v>
       </c>
-      <c r="T7" s="61" t="n">
+      <c r="T7" s="60" t="n">
         <v>95</v>
       </c>
-      <c r="U7" s="61" t="n">
+      <c r="U7" s="60" t="n">
         <v>96</v>
       </c>
-      <c r="V7" s="62" t="n">
+      <c r="V7" s="61" t="n">
         <v>97</v>
       </c>
-      <c r="W7" s="76" t="n">
+      <c r="W7" s="75" t="n">
         <v>98</v>
       </c>
-      <c r="X7" s="61" t="n">
+      <c r="X7" s="60" t="n">
         <v>99</v>
       </c>
-      <c r="Y7" s="77" t="n">
+      <c r="Y7" s="76" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="8" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="81" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="N8" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="79" t="s">
-        <v>45</v>
-      </c>
-      <c r="P8" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="R8" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="S8" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="U8" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="V8" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="X8" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y8" s="79" t="s">
+      <c r="A8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="M8" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="R8" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y8" s="78" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="n">
+      <c r="A9" s="47" t="n">
         <v>101</v>
       </c>
-      <c r="B9" s="41" t="n">
+      <c r="B9" s="40" t="n">
         <v>102</v>
       </c>
-      <c r="C9" s="39" t="n">
+      <c r="C9" s="38" t="n">
         <v>103</v>
       </c>
-      <c r="D9" s="40" t="n">
+      <c r="D9" s="39" t="n">
         <v>104</v>
       </c>
-      <c r="E9" s="61" t="n">
+      <c r="E9" s="60" t="n">
         <v>105</v>
       </c>
-      <c r="F9" s="61" t="n">
+      <c r="F9" s="60" t="n">
         <v>106</v>
       </c>
-      <c r="G9" s="62" t="n">
+      <c r="G9" s="61" t="n">
         <v>107</v>
       </c>
-      <c r="H9" s="76" t="n">
+      <c r="H9" s="75" t="n">
         <v>108</v>
       </c>
-      <c r="I9" s="61" t="n">
+      <c r="I9" s="60" t="n">
         <v>109</v>
       </c>
-      <c r="J9" s="77" t="n">
+      <c r="J9" s="76" t="n">
         <v>110</v>
       </c>
-      <c r="K9" s="48" t="n">
+      <c r="K9" s="47" t="n">
         <v>111</v>
       </c>
-      <c r="L9" s="41" t="n">
+      <c r="L9" s="40" t="n">
         <v>112</v>
       </c>
-      <c r="M9" s="39" t="n">
+      <c r="M9" s="38" t="n">
         <v>113</v>
       </c>
-      <c r="N9" s="40" t="n">
+      <c r="N9" s="39" t="n">
         <v>114</v>
       </c>
-      <c r="O9" s="61" t="n">
+      <c r="O9" s="60" t="n">
         <v>115</v>
       </c>
-      <c r="P9" s="61" t="n">
+      <c r="P9" s="60" t="n">
         <v>116</v>
       </c>
-      <c r="Q9" s="62" t="n">
+      <c r="Q9" s="61" t="n">
         <v>117</v>
       </c>
-      <c r="R9" s="76" t="n">
+      <c r="R9" s="75" t="n">
         <v>118</v>
       </c>
-      <c r="S9" s="61" t="n">
+      <c r="S9" s="60" t="n">
         <v>119</v>
       </c>
-      <c r="T9" s="77" t="n">
+      <c r="T9" s="76" t="n">
         <v>120</v>
       </c>
-      <c r="U9" s="48" t="n">
+      <c r="U9" s="47" t="n">
         <v>121</v>
       </c>
-      <c r="V9" s="41" t="n">
+      <c r="V9" s="40" t="n">
         <v>122</v>
       </c>
-      <c r="W9" s="39" t="n">
+      <c r="W9" s="38" t="n">
         <v>123</v>
       </c>
-      <c r="X9" s="40" t="n">
+      <c r="X9" s="39" t="n">
         <v>124</v>
       </c>
-      <c r="Y9" s="61" t="n">
+      <c r="Y9" s="60" t="n">
         <v>125</v>
       </c>
     </row>
     <row r="10" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="68" t="s">
+      <c r="E10" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="F10" s="68" t="s">
+      <c r="F10" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="69" t="s">
+      <c r="G10" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="68" t="s">
+      <c r="I10" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="J10" s="79" t="s">
+      <c r="J10" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="L10" s="54" t="s">
+      <c r="L10" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="M10" s="55" t="s">
+      <c r="M10" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="N10" s="53" t="s">
+      <c r="N10" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="O10" s="68" t="s">
+      <c r="O10" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="P10" s="68" t="s">
+      <c r="P10" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="Q10" s="69" t="s">
+      <c r="Q10" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="R10" s="78" t="s">
+      <c r="R10" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="S10" s="68" t="s">
+      <c r="S10" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="T10" s="79" t="s">
+      <c r="T10" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="U10" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="V10" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="W10" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="X10" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y10" s="49" t="s">
+      <c r="U10" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="V10" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="W10" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="X10" s="71" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y10" s="48" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="11" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="n">
+      <c r="A11" s="60" t="n">
         <v>126</v>
       </c>
-      <c r="B11" s="62" t="n">
+      <c r="B11" s="61" t="n">
         <v>127</v>
       </c>
-      <c r="C11" s="76" t="n">
+      <c r="C11" s="75" t="n">
         <v>128</v>
       </c>
-      <c r="D11" s="61" t="n">
+      <c r="D11" s="60" t="n">
         <v>129</v>
       </c>
-      <c r="E11" s="77" t="n">
+      <c r="E11" s="76" t="n">
         <v>130</v>
       </c>
-      <c r="F11" s="48" t="n">
+      <c r="F11" s="47" t="n">
         <v>131</v>
       </c>
-      <c r="G11" s="41" t="n">
+      <c r="G11" s="40" t="n">
         <v>132</v>
       </c>
-      <c r="H11" s="39" t="n">
+      <c r="H11" s="38" t="n">
         <v>133</v>
       </c>
-      <c r="I11" s="40" t="n">
+      <c r="I11" s="39" t="n">
         <v>134</v>
       </c>
-      <c r="J11" s="61" t="n">
+      <c r="J11" s="60" t="n">
         <v>135</v>
       </c>
-      <c r="K11" s="61" t="n">
+      <c r="K11" s="60" t="n">
         <v>136</v>
       </c>
-      <c r="L11" s="62" t="n">
+      <c r="L11" s="61" t="n">
         <v>137</v>
       </c>
-      <c r="M11" s="76" t="n">
+      <c r="M11" s="75" t="n">
         <v>138</v>
       </c>
-      <c r="N11" s="61" t="n">
+      <c r="N11" s="60" t="n">
         <v>139</v>
       </c>
-      <c r="O11" s="77" t="n">
+      <c r="O11" s="76" t="n">
         <v>140</v>
       </c>
-      <c r="P11" s="48" t="n">
+      <c r="P11" s="47" t="n">
         <v>141</v>
       </c>
-      <c r="Q11" s="41" t="n">
+      <c r="Q11" s="40" t="n">
         <v>142</v>
       </c>
-      <c r="R11" s="39" t="n">
+      <c r="R11" s="38" t="n">
         <v>143</v>
       </c>
-      <c r="S11" s="40" t="n">
+      <c r="S11" s="39" t="n">
         <v>144</v>
       </c>
-      <c r="T11" s="61" t="n">
+      <c r="T11" s="60" t="n">
         <v>145</v>
       </c>
-      <c r="U11" s="61" t="n">
+      <c r="U11" s="60" t="n">
         <v>146</v>
       </c>
-      <c r="V11" s="62" t="n">
+      <c r="V11" s="61" t="n">
         <v>147</v>
       </c>
-      <c r="W11" s="76" t="n">
+      <c r="W11" s="75" t="n">
         <v>148</v>
       </c>
-      <c r="X11" s="61" t="n">
+      <c r="X11" s="60" t="n">
         <v>149</v>
       </c>
-      <c r="Y11" s="77" t="n">
+      <c r="Y11" s="76" t="n">
         <v>150</v>
       </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="F12" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="J12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="L12" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="M12" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="N12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="O12" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="P12" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q12" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="R12" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="S12" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="T12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="U12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="V12" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="W12" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="X12" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y12" s="79" t="s">
+      <c r="A12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="J12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="O12" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="P12" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q12" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="R12" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="S12" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="T12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="U12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="V12" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="W12" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="X12" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y12" s="78" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="48" t="n">
+      <c r="A13" s="47" t="n">
         <v>151</v>
       </c>
-      <c r="B13" s="41" t="n">
+      <c r="B13" s="40" t="n">
         <v>152</v>
       </c>
-      <c r="C13" s="39" t="n">
+      <c r="C13" s="38" t="n">
         <v>153</v>
       </c>
-      <c r="D13" s="40" t="n">
+      <c r="D13" s="39" t="n">
         <v>154</v>
       </c>
-      <c r="E13" s="61" t="n">
+      <c r="E13" s="60" t="n">
         <v>155</v>
       </c>
-      <c r="F13" s="61" t="n">
+      <c r="F13" s="60" t="n">
         <v>156</v>
       </c>
-      <c r="G13" s="62" t="n">
+      <c r="G13" s="61" t="n">
         <v>157</v>
       </c>
-      <c r="H13" s="76" t="n">
+      <c r="H13" s="75" t="n">
         <v>158</v>
       </c>
-      <c r="I13" s="61" t="n">
+      <c r="I13" s="60" t="n">
         <v>159</v>
       </c>
-      <c r="J13" s="77" t="n">
+      <c r="J13" s="76" t="n">
         <v>160</v>
       </c>
-      <c r="K13" s="48" t="n">
+      <c r="K13" s="47" t="n">
         <v>161</v>
       </c>
-      <c r="L13" s="41" t="n">
+      <c r="L13" s="40" t="n">
         <v>162</v>
       </c>
-      <c r="M13" s="39" t="n">
+      <c r="M13" s="38" t="n">
         <v>163</v>
       </c>
-      <c r="N13" s="40" t="n">
+      <c r="N13" s="39" t="n">
         <v>164</v>
       </c>
-      <c r="O13" s="61" t="n">
+      <c r="O13" s="60" t="n">
         <v>165</v>
       </c>
-      <c r="P13" s="61" t="n">
+      <c r="P13" s="60" t="n">
         <v>166</v>
       </c>
-      <c r="Q13" s="62" t="n">
+      <c r="Q13" s="61" t="n">
         <v>167</v>
       </c>
-      <c r="R13" s="76" t="n">
+      <c r="R13" s="75" t="n">
         <v>168</v>
       </c>
-      <c r="S13" s="61" t="n">
+      <c r="S13" s="60" t="n">
         <v>169</v>
       </c>
-      <c r="T13" s="77" t="n">
+      <c r="T13" s="76" t="n">
         <v>170</v>
       </c>
-      <c r="U13" s="48" t="n">
+      <c r="U13" s="47" t="n">
         <v>171</v>
       </c>
-      <c r="V13" s="41" t="n">
+      <c r="V13" s="40" t="n">
         <v>172</v>
       </c>
-      <c r="W13" s="39" t="n">
+      <c r="W13" s="38" t="n">
         <v>173</v>
       </c>
-      <c r="X13" s="40" t="n">
+      <c r="X13" s="39" t="n">
         <v>174</v>
       </c>
-      <c r="Y13" s="82" t="n">
+      <c r="Y13" s="81" t="n">
         <v>175</v>
       </c>
     </row>
     <row r="14" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="H14" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="J14" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="L14" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="M14" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="N14" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="O14" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="P14" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q14" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="R14" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="S14" s="68" t="s">
-        <v>88</v>
-      </c>
-      <c r="T14" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="U14" s="60" t="s">
+      <c r="A14" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="H14" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="59" t="s">
+        <v>88</v>
+      </c>
+      <c r="L14" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="N14" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="O14" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="P14" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q14" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="R14" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="S14" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="T14" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="U14" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="V14" s="83" t="s">
+      <c r="V14" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="W14" s="84" t="s">
+      <c r="W14" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="X14" s="85" t="s">
+      <c r="X14" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="Y14" s="86" t="s">
+      <c r="Y14" s="85" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="15" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="61" t="n">
+      <c r="A15" s="60" t="n">
         <v>176</v>
       </c>
-      <c r="B15" s="62" t="n">
+      <c r="B15" s="61" t="n">
         <v>177</v>
       </c>
-      <c r="C15" s="63" t="n">
+      <c r="C15" s="62" t="n">
         <v>178</v>
       </c>
-      <c r="D15" s="48" t="n">
+      <c r="D15" s="47" t="n">
         <v>179</v>
       </c>
-      <c r="E15" s="41" t="n">
+      <c r="E15" s="40" t="n">
         <v>180</v>
       </c>
-      <c r="F15" s="39" t="n">
+      <c r="F15" s="38" t="n">
         <v>181</v>
       </c>
-      <c r="G15" s="40" t="n">
+      <c r="G15" s="39" t="n">
         <v>182</v>
       </c>
-      <c r="H15" s="82" t="n">
+      <c r="H15" s="81" t="n">
         <v>183</v>
       </c>
-      <c r="I15" s="61" t="n">
+      <c r="I15" s="60" t="n">
         <v>184</v>
       </c>
-      <c r="J15" s="62" t="n">
+      <c r="J15" s="61" t="n">
         <v>185</v>
       </c>
-      <c r="K15" s="63" t="n">
+      <c r="K15" s="62" t="n">
         <v>186</v>
       </c>
-      <c r="L15" s="48" t="n">
+      <c r="L15" s="47" t="n">
         <v>187</v>
       </c>
-      <c r="M15" s="41" t="n">
+      <c r="M15" s="40" t="n">
         <v>188</v>
       </c>
-      <c r="N15" s="39" t="n">
+      <c r="N15" s="38" t="n">
         <v>189</v>
       </c>
-      <c r="O15" s="40" t="n">
+      <c r="O15" s="39" t="n">
         <v>190</v>
       </c>
-      <c r="P15" s="82" t="n">
+      <c r="P15" s="81" t="n">
         <v>191</v>
       </c>
-      <c r="Q15" s="61" t="n">
+      <c r="Q15" s="60" t="n">
         <v>192</v>
       </c>
-      <c r="R15" s="62" t="n">
+      <c r="R15" s="61" t="n">
         <v>193</v>
       </c>
-      <c r="S15" s="63" t="n">
+      <c r="S15" s="62" t="n">
         <v>194</v>
       </c>
-      <c r="T15" s="48" t="n">
+      <c r="T15" s="47" t="n">
         <v>195</v>
       </c>
-      <c r="U15" s="41" t="n">
+      <c r="U15" s="40" t="n">
         <v>196</v>
       </c>
-      <c r="V15" s="39" t="n">
+      <c r="V15" s="38" t="n">
         <v>197</v>
       </c>
-      <c r="W15" s="40" t="n">
+      <c r="W15" s="39" t="n">
         <v>198</v>
       </c>
-      <c r="X15" s="82" t="n">
+      <c r="X15" s="81" t="n">
         <v>199</v>
       </c>
-      <c r="Y15" s="61" t="n">
+      <c r="Y15" s="60" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="16" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="88" t="s">
+      <c r="C16" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="83" t="s">
+      <c r="E16" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="84" t="s">
+      <c r="F16" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="85" t="s">
+      <c r="G16" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="86" t="s">
+      <c r="H16" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="I16" s="89" t="s">
+      <c r="I16" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="J16" s="87" t="s">
+      <c r="J16" s="86" t="s">
         <v>89</v>
       </c>
-      <c r="K16" s="88" t="s">
+      <c r="K16" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="L16" s="60" t="s">
+      <c r="L16" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="M16" s="83" t="s">
+      <c r="M16" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="N16" s="84" t="s">
+      <c r="N16" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="O16" s="85" t="s">
+      <c r="O16" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="P16" s="86" t="s">
+      <c r="P16" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="89" t="s">
+      <c r="Q16" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="R16" s="87" t="s">
+      <c r="R16" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="S16" s="88" t="s">
+      <c r="S16" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="T16" s="60" t="s">
+      <c r="T16" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="U16" s="54" t="s">
+      <c r="U16" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="V16" s="55" t="s">
+      <c r="V16" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="W16" s="53" t="s">
+      <c r="W16" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="X16" s="90" t="s">
+      <c r="X16" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="Y16" s="68" t="s">
+      <c r="Y16" s="67" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="62" t="n">
+      <c r="A17" s="61" t="n">
         <v>201</v>
       </c>
-      <c r="B17" s="63" t="n">
+      <c r="B17" s="62" t="n">
         <v>202</v>
       </c>
-      <c r="C17" s="48" t="n">
+      <c r="C17" s="47" t="n">
         <v>203</v>
       </c>
-      <c r="D17" s="61" t="n">
+      <c r="D17" s="60" t="n">
         <v>204</v>
       </c>
-      <c r="E17" s="62" t="n">
+      <c r="E17" s="61" t="n">
         <v>205</v>
       </c>
-      <c r="F17" s="76" t="n">
+      <c r="F17" s="75" t="n">
         <v>206</v>
       </c>
-      <c r="G17" s="41" t="n">
+      <c r="G17" s="40" t="n">
         <v>207</v>
       </c>
-      <c r="H17" s="39" t="n">
+      <c r="H17" s="38" t="n">
         <v>208</v>
       </c>
-      <c r="I17" s="40" t="n">
+      <c r="I17" s="39" t="n">
         <v>209</v>
       </c>
-      <c r="J17" s="61" t="n">
+      <c r="J17" s="60" t="n">
         <v>210</v>
       </c>
-      <c r="K17" s="91" t="n">
+      <c r="K17" s="90" t="n">
         <v>211</v>
       </c>
-      <c r="L17" s="92" t="n">
+      <c r="L17" s="91" t="n">
         <v>212</v>
       </c>
-      <c r="M17" s="93" t="n">
+      <c r="M17" s="92" t="n">
         <v>213</v>
       </c>
-      <c r="N17" s="61" t="n">
+      <c r="N17" s="60" t="n">
         <v>214</v>
       </c>
-      <c r="O17" s="62" t="n">
+      <c r="O17" s="61" t="n">
         <v>215</v>
       </c>
-      <c r="P17" s="76" t="n">
+      <c r="P17" s="75" t="n">
         <v>216</v>
       </c>
-      <c r="Q17" s="41" t="n">
+      <c r="Q17" s="40" t="n">
         <v>217</v>
       </c>
-      <c r="R17" s="39" t="n">
+      <c r="R17" s="38" t="n">
         <v>218</v>
       </c>
-      <c r="S17" s="40" t="n">
+      <c r="S17" s="39" t="n">
         <v>219</v>
       </c>
-      <c r="T17" s="61" t="n">
+      <c r="T17" s="60" t="n">
         <v>220</v>
       </c>
-      <c r="U17" s="91" t="n">
+      <c r="U17" s="90" t="n">
         <v>221</v>
       </c>
-      <c r="V17" s="94" t="n">
+      <c r="V17" s="93" t="n">
         <v>222</v>
       </c>
-      <c r="W17" s="95" t="n">
+      <c r="W17" s="94" t="n">
         <v>223</v>
       </c>
-      <c r="X17" s="61" t="n">
+      <c r="X17" s="60" t="n">
         <v>224</v>
       </c>
-      <c r="Y17" s="96" t="n">
+      <c r="Y17" s="95" t="n">
         <v>225</v>
       </c>
     </row>
     <row r="18" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="89" t="s">
+      <c r="D18" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="87" t="s">
+      <c r="E18" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="97" t="s">
+      <c r="F18" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="83" t="s">
+      <c r="G18" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="84" t="s">
+      <c r="H18" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="I18" s="85" t="s">
+      <c r="I18" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="89" t="s">
+      <c r="J18" s="88" t="s">
         <v>90</v>
       </c>
-      <c r="K18" s="98" t="s">
+      <c r="K18" s="97" t="s">
         <v>90</v>
       </c>
-      <c r="L18" s="99" t="s">
+      <c r="L18" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="M18" s="60" t="s">
+      <c r="M18" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="N18" s="89" t="s">
+      <c r="N18" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="O18" s="87" t="s">
+      <c r="O18" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="P18" s="97" t="s">
+      <c r="P18" s="96" t="s">
         <v>91</v>
       </c>
-      <c r="Q18" s="83" t="s">
+      <c r="Q18" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="R18" s="84" t="s">
+      <c r="R18" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="S18" s="85" t="s">
+      <c r="S18" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="T18" s="89" t="s">
+      <c r="T18" s="88" t="s">
         <v>91</v>
       </c>
-      <c r="U18" s="98" t="s">
+      <c r="U18" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="V18" s="100" t="s">
+      <c r="V18" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="W18" s="101" t="s">
+      <c r="W18" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="X18" s="102" t="s">
+      <c r="X18" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="Y18" s="103" t="s">
+      <c r="Y18" s="101" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="19" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="104" t="n">
+      <c r="A19" s="102" t="n">
         <v>226</v>
       </c>
-      <c r="B19" s="41" t="n">
+      <c r="B19" s="40" t="n">
         <v>227</v>
       </c>
-      <c r="C19" s="105" t="n">
+      <c r="C19" s="103" t="n">
         <v>228</v>
       </c>
-      <c r="D19" s="40" t="n">
+      <c r="D19" s="39" t="n">
         <v>229</v>
       </c>
-      <c r="E19" s="61" t="n">
+      <c r="E19" s="60" t="n">
         <v>230</v>
       </c>
-      <c r="F19" s="91" t="n">
+      <c r="F19" s="90" t="n">
         <v>231</v>
       </c>
-      <c r="G19" s="92" t="n">
+      <c r="G19" s="91" t="n">
         <v>232</v>
       </c>
-      <c r="H19" s="106" t="n">
+      <c r="H19" s="104" t="n">
         <v>233</v>
       </c>
-      <c r="I19" s="61" t="n">
+      <c r="I19" s="60" t="n">
         <v>234</v>
       </c>
-      <c r="J19" s="107" t="n">
+      <c r="J19" s="61" t="n">
         <v>235</v>
       </c>
-      <c r="K19" s="76" t="n">
+      <c r="K19" s="75" t="n">
         <v>236</v>
       </c>
-      <c r="L19" s="41" t="n">
+      <c r="L19" s="40" t="n">
         <v>237</v>
       </c>
-      <c r="M19" s="105" t="n">
+      <c r="M19" s="103" t="n">
         <v>238</v>
       </c>
-      <c r="N19" s="40" t="n">
+      <c r="N19" s="39" t="n">
         <v>239</v>
       </c>
-      <c r="O19" s="61" t="n">
+      <c r="O19" s="60" t="n">
         <v>240</v>
       </c>
-      <c r="P19" s="91" t="n">
+      <c r="P19" s="90" t="n">
         <v>241</v>
       </c>
-      <c r="Q19" s="92" t="n">
+      <c r="Q19" s="91" t="n">
         <v>242</v>
       </c>
-      <c r="R19" s="65" t="n">
+      <c r="R19" s="105" t="n">
         <v>243</v>
       </c>
-      <c r="S19" s="65" t="n">
+      <c r="S19" s="60" t="n">
         <v>244</v>
       </c>
-      <c r="T19" s="65" t="n">
+      <c r="T19" s="61" t="n">
         <v>245</v>
       </c>
-      <c r="U19" s="65" t="n">
+      <c r="U19" s="75" t="n">
         <v>246</v>
       </c>
-      <c r="V19" s="65" t="n">
+      <c r="V19" s="40" t="n">
         <v>247</v>
       </c>
-      <c r="W19" s="2" t="n">
+      <c r="W19" s="106" t="n">
         <v>248</v>
       </c>
-      <c r="X19" s="2" t="n">
+      <c r="X19" s="107" t="n">
         <v>249</v>
       </c>
-      <c r="Y19" s="2" t="n">
+      <c r="Y19" s="108" t="n">
         <v>250</v>
       </c>
     </row>
     <row r="20" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="108" t="s">
+      <c r="A20" s="109" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="53" t="s">
         <v>92</v>
       </c>
       <c r="C20" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="111" t="s">
+      <c r="D20" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="102" t="s">
+      <c r="E20" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="112" t="s">
+      <c r="F20" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="G20" s="113" t="s">
+      <c r="G20" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="H20" s="114" t="s">
+      <c r="H20" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="I20" s="102" t="s">
+      <c r="I20" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="115" t="s">
+      <c r="J20" s="114" t="s">
         <v>93</v>
       </c>
-      <c r="K20" s="116" t="s">
+      <c r="K20" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="L20" s="109" t="s">
+      <c r="L20" s="53" t="s">
         <v>93</v>
       </c>
       <c r="M20" s="110" t="s">
         <v>93</v>
       </c>
-      <c r="N20" s="111" t="s">
+      <c r="N20" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="O20" s="102" t="s">
+      <c r="O20" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="P20" s="112" t="s">
+      <c r="P20" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="Q20" s="113" t="s">
+      <c r="Q20" s="112" t="s">
         <v>93</v>
       </c>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
+      <c r="R20" s="113" t="s">
+        <v>94</v>
+      </c>
+      <c r="S20" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="T20" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="U20" s="77" t="s">
+        <v>94</v>
+      </c>
+      <c r="V20" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="W20" s="110" t="s">
+        <v>94</v>
+      </c>
+      <c r="X20" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y20" s="67" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="21" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="n">
+      <c r="A21" s="115" t="n">
         <v>251</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="116" t="n">
         <v>252</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="117" t="n">
         <v>253</v>
       </c>
       <c r="D21" s="2" t="n">
@@ -3597,9 +3629,15 @@
       </c>
     </row>
     <row r="22" s="4" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="111" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="118" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="119" t="s">
+        <v>49</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -4610,103 +4648,103 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="N42" s="117" t="s">
+      <c r="N42" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="O42" s="118" t="s">
-        <v>94</v>
-      </c>
-      <c r="P42" s="119" t="s">
+      <c r="O42" s="121" t="s">
         <v>95</v>
       </c>
-      <c r="Q42" s="120" t="s">
+      <c r="P42" s="122" t="s">
         <v>96</v>
       </c>
-      <c r="R42" s="121" t="s">
+      <c r="Q42" s="123" t="s">
         <v>97</v>
       </c>
-      <c r="S42" s="122" t="s">
+      <c r="R42" s="124" t="s">
         <v>98</v>
       </c>
-      <c r="T42" s="123" t="s">
+      <c r="S42" s="125" t="s">
+        <v>99</v>
+      </c>
+      <c r="T42" s="126" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="124" t="s">
+      <c r="A44" s="127" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="125" t="n">
+      <c r="B44" s="128" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="125" t="n">
+      <c r="C44" s="128" t="n">
         <v>2</v>
       </c>
-      <c r="D44" s="125" t="n">
+      <c r="D44" s="128" t="n">
         <v>3</v>
       </c>
-      <c r="E44" s="125" t="n">
+      <c r="E44" s="128" t="n">
         <v>4</v>
       </c>
-      <c r="F44" s="125" t="n">
+      <c r="F44" s="128" t="n">
         <v>5</v>
       </c>
-      <c r="G44" s="125" t="n">
+      <c r="G44" s="128" t="n">
         <v>6</v>
       </c>
-      <c r="H44" s="125" t="n">
+      <c r="H44" s="128" t="n">
         <v>7</v>
       </c>
-      <c r="I44" s="125" t="n">
+      <c r="I44" s="128" t="n">
         <v>8</v>
       </c>
-      <c r="J44" s="125" t="n">
+      <c r="J44" s="128" t="n">
         <v>9</v>
       </c>
-      <c r="K44" s="126" t="n">
+      <c r="K44" s="129" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="65" t="s">
+      <c r="A45" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="B45" s="127" t="s">
+      <c r="B45" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="128" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="129" t="s">
+      <c r="C45" s="131" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="130" t="s">
+      <c r="D45" s="132" t="s">
         <v>101</v>
       </c>
-      <c r="F45" s="65" t="s">
+      <c r="E45" s="133" t="s">
         <v>102</v>
       </c>
-      <c r="G45" s="131" t="s">
+      <c r="F45" s="64" t="s">
         <v>103</v>
       </c>
-      <c r="H45" s="132" t="s">
+      <c r="G45" s="134" t="s">
+        <v>104</v>
+      </c>
+      <c r="H45" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="65"/>
-      <c r="J45" s="65"/>
-      <c r="K45" s="65"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="64"/>
       <c r="L45" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M45" s="133" t="s">
         <v>105</v>
       </c>
-      <c r="N45" s="133"/>
-      <c r="O45" s="133" t="s">
+      <c r="M45" s="136" t="s">
         <v>106</v>
       </c>
-      <c r="P45" s="133"/>
+      <c r="N45" s="136"/>
+      <c r="O45" s="136" t="s">
+        <v>107</v>
+      </c>
+      <c r="P45" s="136"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
@@ -4715,90 +4753,90 @@
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" s="36" t="s">
+      <c r="C46" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="E46" s="45" t="s">
+      <c r="D46" s="35" t="s">
         <v>101</v>
       </c>
+      <c r="E46" s="44" t="s">
+        <v>102</v>
+      </c>
       <c r="F46" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H46" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="I46" s="134" t="s">
+      <c r="H46" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="I46" s="137" t="s">
         <v>38</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L46" s="135" t="s">
         <v>110</v>
       </c>
-      <c r="M46" s="135"/>
-      <c r="N46" s="135"/>
-      <c r="O46" s="133" t="s">
+      <c r="L46" s="138" t="s">
         <v>111</v>
       </c>
-      <c r="P46" s="133"/>
-      <c r="Q46" s="133"/>
-      <c r="R46" s="133" t="s">
+      <c r="M46" s="138"/>
+      <c r="N46" s="138"/>
+      <c r="O46" s="136" t="s">
         <v>112</v>
       </c>
-      <c r="S46" s="133"/>
+      <c r="P46" s="136"/>
+      <c r="Q46" s="136"/>
+      <c r="R46" s="136" t="s">
+        <v>113</v>
+      </c>
+      <c r="S46" s="136"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" s="36" t="s">
+      <c r="C47" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="E47" s="45" t="s">
+      <c r="D47" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="F47" s="14" t="s">
-        <v>113</v>
+      <c r="E47" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H47" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="I47" s="134" t="s">
+      <c r="H47" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="I47" s="137" t="s">
         <v>38</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="135" t="s">
-        <v>114</v>
-      </c>
-      <c r="M47" s="135"/>
+      <c r="L47" s="138" t="s">
+        <v>115</v>
+      </c>
+      <c r="M47" s="138"/>
       <c r="N47" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
@@ -4806,56 +4844,56 @@
       <c r="S47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" s="43" t="s">
+      <c r="A48" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="136" t="s">
+      <c r="C48" s="139" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="H48" s="140" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="134" t="s">
-        <v>38</v>
-      </c>
-      <c r="F48" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="G48" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="H48" s="137" t="s">
-        <v>101</v>
-      </c>
       <c r="I48" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J48" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="K48" s="138" t="s">
+        <v>114</v>
+      </c>
+      <c r="J48" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="K48" s="141" t="s">
+        <v>120</v>
+      </c>
       <c r="L48" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="M48" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N48" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O48" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P48" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q48" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>